<commit_message>
added 3 motors to the microBoSL in schematic and PCB, traces and silkscreen still need optimising
</commit_message>
<xml_diff>
--- a/micro/EDA/microBoSL BOM Rev 0.2.0.xlsx
+++ b/micro/EDA/microBoSL BOM Rev 0.2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.monash.edu\home\User070\scat0009\Documents\Repositories\BoSL-nano\micro\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A10653-338D-48EC-9C97-C69F950049CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16776856-89C9-4651-ACC8-507B6807DCE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -859,7 +859,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
routed pcb with 4 hall effect sensors, TODO silkscreen
</commit_message>
<xml_diff>
--- a/micro/EDA/microBoSL BOM Rev 0.2.0.xlsx
+++ b/micro/EDA/microBoSL BOM Rev 0.2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.monash.edu\home\User070\scat0009\Documents\Repositories\BoSL-nano\micro\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16776856-89C9-4651-ACC8-507B6807DCE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E054F66-987B-408C-A56C-E3CB25B516A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -859,13 +859,14 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
-    <col min="2" max="3" width="20.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" customWidth="1"/>
@@ -1483,14 +1484,14 @@
         <v>75</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J16" s="7">
         <v>1.55</v>
       </c>
       <c r="K16" s="7">
         <f t="shared" si="0"/>
-        <v>1.55</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>113</v>

</xml_diff>